<commit_message>
Rend accessible le fichier de carrières
</commit_message>
<xml_diff>
--- a/demo/carrieres.xlsx
+++ b/demo/carrieres.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t xml:space="preserve">description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">titre</t>
   </si>
   <si>
     <t xml:space="preserve">SMIC</t>
@@ -45,10 +48,16 @@
     <t xml:space="preserve">Salaire moyen par tête de base</t>
   </si>
   <si>
+    <t xml:space="preserve">Salaire moyen</t>
+  </si>
+  <si>
     <t xml:space="preserve">COR1</t>
   </si>
   <si>
     <t xml:space="preserve">Cas type n°1 du COR (cadre à carrière sans interruption)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cadre sans interruption de carrière </t>
   </si>
   <si>
     <t xml:space="preserve">COR2</t>
@@ -57,10 +66,16 @@
     <t xml:space="preserve">Cas type n°2 du COR (non cadre à carrière sans interruption)</t>
   </si>
   <si>
+    <t xml:space="preserve">Non cadre sans interruption de carrière </t>
+  </si>
+  <si>
     <t xml:space="preserve">COR3</t>
   </si>
   <si>
     <t xml:space="preserve">Cas type n°3 du COR (non cadre à carrière interrompue par du chômage )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non cadre à carrière interrompue par du chômage</t>
   </si>
   <si>
     <t xml:space="preserve">COR4</t>
@@ -69,7 +84,13 @@
     <t xml:space="preserve">Cas type n°4 du COR (non cadre avec une interruption de carrière pour enfant)</t>
   </si>
   <si>
+    <t xml:space="preserve">Non cadre avec une interruption de carrière pour enfant</t>
+  </si>
+  <si>
     <t xml:space="preserve">PlafondSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plafond de la sécurité sociale</t>
   </si>
   <si>
     <t xml:space="preserve">age</t>
@@ -85,7 +106,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -106,6 +127,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -150,12 +176,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -176,10 +206,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -197,82 +227,106 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -304,25 +358,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2875,19 +2929,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>